<commit_message>
Convert to Range and Subtotaling
</commit_message>
<xml_diff>
--- a/Intermediate I/Week 5/workbook/W5_V5 ConvertAndSubtotal.xlsx
+++ b/Intermediate I/Week 5/workbook/W5_V5 ConvertAndSubtotal.xlsx
@@ -1,56 +1,78 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
-  <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mq31837921/Google Drive/Excel MOOC/002 Course 2 - Intermediate I/05 Week 5/01 Workbooks/Actual Recorded/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF953F6-C702-4055-B0CC-9A9AC780B719}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28380" windowHeight="15480"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="1" r:id="rId1"/>
     <sheet name="Stats" sheetId="2" r:id="rId2"/>
+    <sheet name="Staff (2)" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Staff!$A$4:$H$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Staff (2)'!$A$4:$H$30</definedName>
+    <definedName name="Annual_Salary" localSheetId="2">'Staff (2)'!$N$4:$N$46</definedName>
     <definedName name="Annual_Salary">Staff!$N$4:$N$39</definedName>
+    <definedName name="Date_of_Hire" localSheetId="2">'Staff (2)'!$F$4:$F$46</definedName>
     <definedName name="Date_of_Hire">Staff!$F$4:$F$39</definedName>
+    <definedName name="Department" localSheetId="2">'Staff (2)'!$H$4:$H$46</definedName>
     <definedName name="Department">Staff!$H$4:$H$39</definedName>
+    <definedName name="Email" localSheetId="2">'Staff (2)'!$E$4:$E$46</definedName>
     <definedName name="Email">Staff!$E$4:$E$39</definedName>
+    <definedName name="Emp_ID" localSheetId="2">'Staff (2)'!$A$4:$A$46</definedName>
     <definedName name="Emp_ID">Staff!$A$4:$A$39</definedName>
+    <definedName name="Extension" localSheetId="2">'Staff (2)'!$K$4:$K$46</definedName>
     <definedName name="Extension">Staff!$K$4:$K$39</definedName>
+    <definedName name="First" localSheetId="2">'Staff (2)'!$C$4:$C$46</definedName>
     <definedName name="First">Staff!$C$4:$C$39</definedName>
+    <definedName name="Floor" localSheetId="2">'Staff (2)'!$J$4:$J$46</definedName>
     <definedName name="Floor">Staff!$J$4:$J$39</definedName>
+    <definedName name="Gender" localSheetId="2">'Staff (2)'!$D$4:$D$46</definedName>
     <definedName name="Gender">Staff!$D$4:$D$39</definedName>
+    <definedName name="Last" localSheetId="2">'Staff (2)'!$B$4:$B$46</definedName>
     <definedName name="Last">Staff!$B$4:$B$39</definedName>
+    <definedName name="Last_Review" localSheetId="2">'Staff (2)'!$L$4:$L$46</definedName>
     <definedName name="Last_Review">Staff!$L$4:$L$39</definedName>
+    <definedName name="Location" localSheetId="2">'Staff (2)'!$I$4:$I$46</definedName>
     <definedName name="Location">Staff!$I$4:$I$39</definedName>
+    <definedName name="Next_Review" localSheetId="2">'Staff (2)'!$M$4:$M$46</definedName>
     <definedName name="Next_Review">Staff!$M$4:$M$39</definedName>
+    <definedName name="Pension" localSheetId="2">'Staff (2)'!$O$4:$O$46</definedName>
     <definedName name="Pension">Staff!$O$4:$O$39</definedName>
+    <definedName name="Pension_Rate" localSheetId="2">'Staff (2)'!$P$1</definedName>
     <definedName name="Pension_Rate">Staff!$P$1</definedName>
+    <definedName name="Years_Service" localSheetId="2">'Staff (2)'!$G$4:$G$46</definedName>
     <definedName name="Years_Service">Staff!$G$4:$G$39</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="185">
   <si>
     <t>Emp ID</t>
   </si>
@@ -578,19 +600,46 @@
   </si>
   <si>
     <t>Marketing</t>
+  </si>
+  <si>
+    <t>Accounting Total</t>
+  </si>
+  <si>
+    <t>Customer Service Total</t>
+  </si>
+  <si>
+    <t>Executive Total</t>
+  </si>
+  <si>
+    <t>Facilities Total</t>
+  </si>
+  <si>
+    <t>Human Resources Total</t>
+  </si>
+  <si>
+    <t>IT Total</t>
+  </si>
+  <si>
+    <t>Marketing Total</t>
+  </si>
+  <si>
+    <t>Sales Total</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -654,8 +703,23 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -678,8 +742,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -702,6 +772,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -710,7 +789,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -778,6 +857,71 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -787,129 +931,6 @@
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
   <dxfs count="37">
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -972,7 +993,27 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -980,11 +1021,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1037,10 +1087,65 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1081,7 +1186,46 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1103,9 +1247,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1117,7 +1261,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1207,7 +1350,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-E128-4193-9B57-C543C5AE0055}"/>
               </c:ext>
@@ -1254,7 +1397,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-E128-4193-9B57-C543C5AE0055}"/>
               </c:ext>
@@ -1312,10 +1455,8 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1339,15 +1480,15 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-421C-4D93-A2C2-316304DC4BC2}"/>
             </c:ext>
@@ -1375,7 +1516,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1443,9 +1583,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1457,7 +1597,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1547,7 +1686,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-6DAF-468C-822C-65D9136E4819}"/>
               </c:ext>
@@ -1594,7 +1733,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-6DAF-468C-822C-65D9136E4819}"/>
               </c:ext>
@@ -1641,7 +1780,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-6DAF-468C-822C-65D9136E4819}"/>
               </c:ext>
@@ -1688,7 +1827,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-6DAF-468C-822C-65D9136E4819}"/>
               </c:ext>
@@ -1735,7 +1874,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-6DAF-468C-822C-65D9136E4819}"/>
               </c:ext>
@@ -1782,7 +1921,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-6DAF-468C-822C-65D9136E4819}"/>
               </c:ext>
@@ -1832,6 +1971,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-77BA-472D-BAAB-822CF24F9A8E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1885,10 +2029,8 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1927,30 +2069,30 @@
                 <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>197800.0</c:v>
+                  <c:v>197800</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>278500.0</c:v>
+                  <c:v>278500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>807000.0</c:v>
+                  <c:v>807000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>255500.0</c:v>
+                  <c:v>255500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>227800.0</c:v>
+                  <c:v>227800</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>149700.0</c:v>
+                  <c:v>149700</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>97000.0</c:v>
+                  <c:v>97000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-85D7-4AB5-A501-7B32B63B91A1}"/>
             </c:ext>
@@ -1978,7 +2120,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3149,7 +3290,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8DB5471F-1593-40AB-B7CD-50B21DB329DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DB5471F-1593-40AB-B7CD-50B21DB329DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3185,7 +3326,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEA7632C-135D-4CE6-B2B6-50468D13BE85}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEA7632C-135D-4CE6-B2B6-50468D13BE85}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3207,40 +3348,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:P40" totalsRowCount="1" dataDxfId="36">
-  <autoFilter ref="A3:P39"/>
-  <sortState ref="A4:O38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:P40" totalsRowCount="1" dataDxfId="36">
+  <autoFilter ref="A3:P39" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:O38">
     <sortCondition ref="A3:A38"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" name="Emp ID" totalsRowFunction="count" dataDxfId="35" totalsRowDxfId="15"/>
-    <tableColumn id="2" name="Last"/>
-    <tableColumn id="3" name="First" dataDxfId="34" totalsRowDxfId="14"/>
-    <tableColumn id="4" name="Gender" dataDxfId="33" totalsRowDxfId="13"/>
-    <tableColumn id="5" name="Email">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Emp ID" totalsRowFunction="count" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Last"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="First" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Gender" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Email">
       <calculatedColumnFormula>LOWER(C4&amp;"."&amp;B4&amp;"@pushpin.com")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Date of Hire" dataDxfId="32" totalsRowDxfId="12"/>
-    <tableColumn id="7" name="Years Service" totalsRowFunction="average" dataDxfId="31" totalsRowDxfId="11">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date of Hire" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Years Service" totalsRowFunction="average" dataDxfId="27" totalsRowDxfId="26">
       <calculatedColumnFormula>YEARFRAC(F4,TODAY())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Department" dataDxfId="30" totalsRowDxfId="10"/>
-    <tableColumn id="9" name="Location" dataDxfId="29" totalsRowDxfId="9"/>
-    <tableColumn id="10" name="Floor" dataDxfId="28" totalsRowDxfId="8">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Department" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Location" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Floor" dataDxfId="21" totalsRowDxfId="20">
       <calculatedColumnFormula>LEFT(I4,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Extension" dataDxfId="27" totalsRowDxfId="7">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Extension" dataDxfId="19" totalsRowDxfId="18">
       <calculatedColumnFormula>RIGHT(I4,4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Last Review" dataDxfId="26" totalsRowDxfId="6"/>
-    <tableColumn id="13" name="Next Review" dataDxfId="25" totalsRowDxfId="5">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Last Review" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Next Review" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>L4+365</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Annual Salary" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="4"/>
-    <tableColumn id="15" name="Pension" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="3">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Annual Salary" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Pension" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>N4*Pension_Rate</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Package" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="2">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Package" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[Annual Salary]:[Pension]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3249,22 +3390,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A15:D22" totalsRowShown="0">
-  <autoFilter ref="A15:D22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A15:D22" totalsRowShown="0">
+  <autoFilter ref="A15:D22" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="Department" dataDxfId="23"/>
-    <tableColumn id="2" name="Total Salary" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Department" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Total Salary" dataDxfId="6">
       <calculatedColumnFormula>SUMIFS(Annual_Salary,Department,A16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="M" dataDxfId="21">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="M" dataDxfId="5">
       <calculatedColumnFormula>SUMIFS(Annual_Salary,Department,A16,Gender,$C$15)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="F" dataDxfId="20">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="F" dataDxfId="4">
       <calculatedColumnFormula>SUMIFS(Annual_Salary,Department,A16,Gender,$D$15)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3568,34 +3709,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="3" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="3" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
-    <col min="9" max="9" width="16.1640625" customWidth="1"/>
-    <col min="10" max="10" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" customWidth="1"/>
-    <col min="12" max="12" width="14.1640625" customWidth="1"/>
-    <col min="13" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="14" width="15.1640625" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" customWidth="1"/>
+    <col min="8" max="8" width="17.6328125" customWidth="1"/>
+    <col min="9" max="9" width="16.1796875" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" customWidth="1"/>
+    <col min="12" max="12" width="14.1796875" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" customWidth="1"/>
+    <col min="14" max="14" width="15.1796875" customWidth="1"/>
+    <col min="15" max="15" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A1" s="18" t="s">
         <v>95</v>
       </c>
@@ -3606,7 +3747,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3656,7 +3797,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -3678,7 +3819,7 @@
       </c>
       <c r="G4" s="4">
         <f t="shared" ref="G4:G38" ca="1" si="1">YEARFRAC(F4,TODAY())</f>
-        <v>16.547222222222221</v>
+        <v>19.380555555555556</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>22</v>
@@ -3713,7 +3854,7 @@
         <v>110526</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -3735,7 +3876,7 @@
       </c>
       <c r="G5" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>16.475000000000001</v>
+        <v>19.308333333333334</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>59</v>
@@ -3770,7 +3911,7 @@
         <v>76627</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -3792,7 +3933,7 @@
       </c>
       <c r="G6" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>14.936111111111112</v>
+        <v>17.769444444444446</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>55</v>
@@ -3827,7 +3968,7 @@
         <v>74992</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>63</v>
       </c>
@@ -3849,7 +3990,7 @@
       </c>
       <c r="G7" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>13.322222222222223</v>
+        <v>16.155555555555555</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>24</v>
@@ -3884,7 +4025,7 @@
         <v>64528</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>64</v>
       </c>
@@ -3906,7 +4047,7 @@
       </c>
       <c r="G8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>12.091666666666667</v>
+        <v>14.925000000000001</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>55</v>
@@ -3941,7 +4082,7 @@
         <v>68561</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>65</v>
       </c>
@@ -3963,7 +4104,7 @@
       </c>
       <c r="G9" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>11.558333333333334</v>
+        <v>14.391666666666667</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>24</v>
@@ -3998,7 +4139,7 @@
         <v>63656</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>66</v>
       </c>
@@ -4020,7 +4161,7 @@
       </c>
       <c r="G10" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>11.405555555555555</v>
+        <v>14.238888888888889</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>55</v>
@@ -4055,7 +4196,7 @@
         <v>64528</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>67</v>
       </c>
@@ -4077,7 +4218,7 @@
       </c>
       <c r="G11" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>10.794444444444444</v>
+        <v>13.627777777777778</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>15</v>
@@ -4112,7 +4253,7 @@
         <v>56244</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>68</v>
       </c>
@@ -4134,7 +4275,7 @@
       </c>
       <c r="G12" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3472222222222214</v>
+        <v>12.180555555555555</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>55</v>
@@ -4169,7 +4310,7 @@
         <v>63438</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>69</v>
       </c>
@@ -4191,7 +4332,7 @@
       </c>
       <c r="G13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>8.9777777777777779</v>
+        <v>11.811111111111112</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>24</v>
@@ -4226,7 +4367,7 @@
         <v>60822</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>70</v>
       </c>
@@ -4248,7 +4389,7 @@
       </c>
       <c r="G14" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>7.6805555555555554</v>
+        <v>10.513888888888889</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>55</v>
@@ -4283,7 +4424,7 @@
         <v>60495</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>71</v>
       </c>
@@ -4305,7 +4446,7 @@
       </c>
       <c r="G15" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5194444444444448</v>
+        <v>10.352777777777778</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>59</v>
@@ -4340,7 +4481,7 @@
         <v>52756</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>72</v>
       </c>
@@ -4362,7 +4503,7 @@
       </c>
       <c r="G16" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4916666666666663</v>
+        <v>9.3249999999999993</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>55</v>
@@ -4397,7 +4538,7 @@
         <v>64637</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>73</v>
       </c>
@@ -4419,7 +4560,7 @@
       </c>
       <c r="G17" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1638888888888888</v>
+        <v>8.9972222222222218</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>55</v>
@@ -4454,7 +4595,7 @@
         <v>61040</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>74</v>
       </c>
@@ -4476,7 +4617,7 @@
       </c>
       <c r="G18" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3944444444444448</v>
+        <v>8.2277777777777779</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>17</v>
@@ -4511,7 +4652,7 @@
         <v>68888</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>75</v>
       </c>
@@ -4533,7 +4674,7 @@
       </c>
       <c r="G19" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9027777777777777</v>
+        <v>7.7361111111111107</v>
       </c>
       <c r="H19" t="s">
         <v>59</v>
@@ -4568,7 +4709,7 @@
         <v>56353</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>76</v>
       </c>
@@ -4590,7 +4731,7 @@
       </c>
       <c r="G20" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8055555555555554</v>
+        <v>7.6388888888888893</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>59</v>
@@ -4625,7 +4766,7 @@
         <v>54064</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>77</v>
       </c>
@@ -4647,7 +4788,7 @@
       </c>
       <c r="G21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2805555555555559</v>
+        <v>7.1138888888888889</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>24</v>
@@ -4682,7 +4823,7 @@
         <v>49159</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>78</v>
       </c>
@@ -4704,7 +4845,7 @@
       </c>
       <c r="G22" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2222222222222223</v>
+        <v>6.0555555555555554</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>13</v>
@@ -4739,7 +4880,7 @@
         <v>45889</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
@@ -4761,7 +4902,7 @@
       </c>
       <c r="G23" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9361111111111109</v>
+        <v>5.7694444444444448</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>15</v>
@@ -4796,7 +4937,7 @@
         <v>68452</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>80</v>
       </c>
@@ -4818,7 +4959,7 @@
       </c>
       <c r="G24" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9083333333333332</v>
+        <v>5.7416666666666663</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>55</v>
@@ -4853,7 +4994,7 @@
         <v>59623</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>81</v>
       </c>
@@ -4875,7 +5016,7 @@
       </c>
       <c r="G25" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7638888888888888</v>
+        <v>5.5972222222222223</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>55</v>
@@ -4910,7 +5051,7 @@
         <v>57334</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>82</v>
       </c>
@@ -4932,7 +5073,7 @@
       </c>
       <c r="G26" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6722222222222221</v>
+        <v>5.5055555555555555</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>15</v>
@@ -4967,7 +5108,7 @@
         <v>63765</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>83</v>
       </c>
@@ -4989,7 +5130,7 @@
       </c>
       <c r="G27" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6361111111111111</v>
+        <v>5.4694444444444441</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>55</v>
@@ -5024,7 +5165,7 @@
         <v>50685</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>84</v>
       </c>
@@ -5046,7 +5187,7 @@
       </c>
       <c r="G28" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3111111111111109</v>
+        <v>5.1444444444444448</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>55</v>
@@ -5081,7 +5222,7 @@
         <v>61258</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>85</v>
       </c>
@@ -5103,7 +5244,7 @@
       </c>
       <c r="G29" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0166666666666666</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>15</v>
@@ -5138,7 +5279,7 @@
         <v>59841</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>86</v>
       </c>
@@ -5160,7 +5301,7 @@
       </c>
       <c r="G30" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0138888888888888</v>
+        <v>4.8472222222222223</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>17</v>
@@ -5195,7 +5336,7 @@
         <v>52211</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>87</v>
       </c>
@@ -5217,7 +5358,7 @@
       </c>
       <c r="G31" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7638888888888888</v>
+        <v>4.5972222222222223</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>55</v>
@@ -5252,7 +5393,7 @@
         <v>54064</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>88</v>
       </c>
@@ -5274,7 +5415,7 @@
       </c>
       <c r="G32" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7555555555555555</v>
+        <v>4.5888888888888886</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>55</v>
@@ -5309,7 +5450,7 @@
         <v>38804</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>89</v>
       </c>
@@ -5331,7 +5472,7 @@
       </c>
       <c r="G33" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6277777777777778</v>
+        <v>4.4611111111111112</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>59</v>
@@ -5366,7 +5507,7 @@
         <v>63765</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>90</v>
       </c>
@@ -5388,7 +5529,7 @@
       </c>
       <c r="G34" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5916666666666666</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>55</v>
@@ -5423,7 +5564,7 @@
         <v>56026</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>91</v>
       </c>
@@ -5445,7 +5586,7 @@
       </c>
       <c r="G35" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.75277777777777777</v>
+        <v>3.5861111111111112</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>17</v>
@@ -5480,7 +5621,7 @@
         <v>42074</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>92</v>
       </c>
@@ -5502,7 +5643,7 @@
       </c>
       <c r="G36" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6694444444444444</v>
+        <v>3.5027777777777778</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>55</v>
@@ -5537,7 +5678,7 @@
         <v>44145</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>93</v>
       </c>
@@ -5559,7 +5700,7 @@
       </c>
       <c r="G37" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>7.6055555555555552</v>
+        <v>10.438888888888888</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>22</v>
@@ -5594,7 +5735,7 @@
         <v>105076</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>94</v>
       </c>
@@ -5616,7 +5757,7 @@
       </c>
       <c r="G38" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24722222222222223</v>
+        <v>3.0805555555555557</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>24</v>
@@ -5651,7 +5792,7 @@
         <v>40330</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>172</v>
       </c>
@@ -5673,7 +5814,7 @@
       </c>
       <c r="G39" s="4">
         <f ca="1">YEARFRAC(F39,TODAY())</f>
-        <v>8.611111111111111E-2</v>
+        <v>2.9194444444444443</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>175</v>
@@ -5706,7 +5847,7 @@
         <v>105730</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <f>SUBTOTAL(103,Table1[Emp ID])</f>
         <v>36</v>
@@ -5715,7 +5856,7 @@
       <c r="D40" s="19"/>
       <c r="G40" s="4">
         <f ca="1">SUBTOTAL(101,Table1[Years Service])</f>
-        <v>5.896527777777778</v>
+        <v>8.7298611111111128</v>
       </c>
       <c r="H40" s="21"/>
       <c r="I40" s="22"/>
@@ -5736,24 +5877,24 @@
         <v>2240386</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E42" s="13"/>
     </row>
-    <row r="43" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E43" s="13"/>
     </row>
-    <row r="44" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E44" s="13"/>
     </row>
   </sheetData>
-  <sortState ref="A4:N38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:N38">
     <sortCondition ref="A7"/>
   </sortState>
   <conditionalFormatting sqref="M4:M39">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>M4&lt;TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5766,28 +5907,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1"/>
-    <col min="2" max="4" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.6328125" customWidth="1"/>
+    <col min="2" max="4" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A1" s="18" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>162</v>
       </c>
@@ -5796,7 +5937,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>134</v>
       </c>
@@ -5805,7 +5946,7 @@
         <v>2055400</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>135</v>
       </c>
@@ -5814,16 +5955,16 @@
         <v>57094.444444444445</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>136</v>
       </c>
       <c r="B6" s="11">
         <f ca="1">MAX(Years_Service)</f>
-        <v>16.547222222222221</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>19.380555555555556</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>137</v>
       </c>
@@ -5832,7 +5973,7 @@
         <v>42933</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>164</v>
       </c>
@@ -5840,7 +5981,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>168</v>
       </c>
@@ -5849,7 +5990,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>169</v>
       </c>
@@ -5858,7 +5999,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -5872,7 +6013,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -5889,7 +6030,7 @@
         <v>96400</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
@@ -5906,7 +6047,7 @@
         <v>100100</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>55</v>
       </c>
@@ -5923,7 +6064,7 @@
         <v>411400</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -5940,7 +6081,7 @@
         <v>196300</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -5957,7 +6098,7 @@
         <v>113400</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -5974,7 +6115,7 @@
         <v>63200</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="21" t="s">
         <v>175</v>
       </c>
@@ -5999,4 +6140,2428 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E879B68D-D327-4F2D-9F9A-050148ED851E}">
+  <dimension ref="A1:P52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" outlineLevelRow="2" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.1796875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" customWidth="1"/>
+    <col min="8" max="8" width="17.6328125" customWidth="1"/>
+    <col min="9" max="9" width="16.1796875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.1796875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1796875" customWidth="1"/>
+    <col min="15" max="15" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="28.5" x14ac:dyDescent="0.65">
+      <c r="A1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="P1" s="15">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="M3" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="N3" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="O3" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="P3" s="26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A4" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="28" t="str">
+        <f>LOWER(C4&amp;"."&amp;B4&amp;"@pushpin.com")</f>
+        <v>nicholas.fernandes@pushpin.com</v>
+      </c>
+      <c r="F4" s="31">
+        <v>39023</v>
+      </c>
+      <c r="G4" s="32">
+        <f ca="1">YEARFRAC(F4,TODAY())</f>
+        <v>13.627777777777778</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="J4" s="35" t="str">
+        <f>LEFT(I4,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K4" s="35" t="str">
+        <f>RIGHT(I4,4)</f>
+        <v>2372</v>
+      </c>
+      <c r="L4" s="31">
+        <v>42614</v>
+      </c>
+      <c r="M4" s="31">
+        <f>L4+365</f>
+        <v>42979</v>
+      </c>
+      <c r="N4" s="36">
+        <v>51600</v>
+      </c>
+      <c r="O4" s="37">
+        <f>N4*Pension_Rate</f>
+        <v>4644</v>
+      </c>
+      <c r="P4" s="38">
+        <f>SUM('Staff (2)'!$N4:$O4)</f>
+        <v>56244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A5" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E5" s="25" t="str">
+        <f>LOWER(C5&amp;"."&amp;B5&amp;"@pushpin.com")</f>
+        <v>jim.boller@pushpin.com</v>
+      </c>
+      <c r="F5" s="40">
+        <v>41893</v>
+      </c>
+      <c r="G5" s="41">
+        <f ca="1">YEARFRAC(F5,TODAY())</f>
+        <v>5.7694444444444448</v>
+      </c>
+      <c r="H5" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="J5" s="44" t="str">
+        <f>LEFT(I5,2)</f>
+        <v>03</v>
+      </c>
+      <c r="K5" s="44" t="str">
+        <f>RIGHT(I5,4)</f>
+        <v>2318</v>
+      </c>
+      <c r="L5" s="40">
+        <v>42835</v>
+      </c>
+      <c r="M5" s="40">
+        <f>L5+365</f>
+        <v>43200</v>
+      </c>
+      <c r="N5" s="45">
+        <v>62800</v>
+      </c>
+      <c r="O5" s="46">
+        <f>N5*Pension_Rate</f>
+        <v>5652</v>
+      </c>
+      <c r="P5" s="47">
+        <f>SUM('Staff (2)'!$N5:$O5)</f>
+        <v>68452</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A6" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="25" t="str">
+        <f>LOWER(C6&amp;"."&amp;B6&amp;"@pushpin.com")</f>
+        <v>anna.clark@pushpin.com</v>
+      </c>
+      <c r="F6" s="40">
+        <v>41989</v>
+      </c>
+      <c r="G6" s="41">
+        <f ca="1">YEARFRAC(F6,TODAY())</f>
+        <v>5.5055555555555555</v>
+      </c>
+      <c r="H6" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="44" t="str">
+        <f>LEFT(I6,2)</f>
+        <v>03</v>
+      </c>
+      <c r="K6" s="44" t="str">
+        <f>RIGHT(I6,4)</f>
+        <v>2601</v>
+      </c>
+      <c r="L6" s="40">
+        <v>42731</v>
+      </c>
+      <c r="M6" s="40">
+        <f>L6+365</f>
+        <v>43096</v>
+      </c>
+      <c r="N6" s="45">
+        <v>58500</v>
+      </c>
+      <c r="O6" s="46">
+        <f>N6*Pension_Rate</f>
+        <v>5265</v>
+      </c>
+      <c r="P6" s="47">
+        <f>SUM('Staff (2)'!$N6:$O6)</f>
+        <v>63765</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A7" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="25" t="str">
+        <f>LOWER(C7&amp;"."&amp;B7&amp;"@pushpin.com")</f>
+        <v>alexandra.donnell@pushpin.com</v>
+      </c>
+      <c r="F7" s="40">
+        <v>42228</v>
+      </c>
+      <c r="G7" s="41">
+        <f ca="1">YEARFRAC(F7,TODAY())</f>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="H7" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="J7" s="44" t="str">
+        <f>LEFT(I7,2)</f>
+        <v>03</v>
+      </c>
+      <c r="K7" s="44" t="str">
+        <f>RIGHT(I7,4)</f>
+        <v>2082</v>
+      </c>
+      <c r="L7" s="40">
+        <v>42629</v>
+      </c>
+      <c r="M7" s="40">
+        <f>L7+365</f>
+        <v>42994</v>
+      </c>
+      <c r="N7" s="45">
+        <v>54900</v>
+      </c>
+      <c r="O7" s="46">
+        <f>N7*Pension_Rate</f>
+        <v>4941</v>
+      </c>
+      <c r="P7" s="47">
+        <f>SUM('Staff (2)'!$N7:$O7)</f>
+        <v>59841</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="39"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="I8" s="43"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="45">
+        <f>SUBTOTAL(9,N4:N7)</f>
+        <v>227800</v>
+      </c>
+      <c r="O8" s="46">
+        <f>SUBTOTAL(9,O4:O7)</f>
+        <v>20502</v>
+      </c>
+      <c r="P8" s="47">
+        <f>SUBTOTAL(9,P4:P7)</f>
+        <v>248302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A9" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9" s="25" t="str">
+        <f>LOWER(C9&amp;"."&amp;B9&amp;"@pushpin.com")</f>
+        <v>adam.barry@pushpin.com</v>
+      </c>
+      <c r="F9" s="40">
+        <v>38099</v>
+      </c>
+      <c r="G9" s="41">
+        <f ca="1">YEARFRAC(F9,TODAY())</f>
+        <v>16.155555555555555</v>
+      </c>
+      <c r="H9" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" s="44" t="str">
+        <f>LEFT(I9,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K9" s="44" t="str">
+        <f>RIGHT(I9,4)</f>
+        <v>2018</v>
+      </c>
+      <c r="L9" s="40">
+        <v>42860</v>
+      </c>
+      <c r="M9" s="40">
+        <f>L9+365</f>
+        <v>43225</v>
+      </c>
+      <c r="N9" s="45">
+        <v>59200</v>
+      </c>
+      <c r="O9" s="46">
+        <f>N9*Pension_Rate</f>
+        <v>5328</v>
+      </c>
+      <c r="P9" s="47">
+        <f>SUM('Staff (2)'!$N9:$O9)</f>
+        <v>64528</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A10" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10" s="25" t="str">
+        <f>LOWER(C10&amp;"."&amp;B10&amp;"@pushpin.com")</f>
+        <v>susan.filosa@pushpin.com</v>
+      </c>
+      <c r="F10" s="40">
+        <v>38744</v>
+      </c>
+      <c r="G10" s="41">
+        <f ca="1">YEARFRAC(F10,TODAY())</f>
+        <v>14.391666666666667</v>
+      </c>
+      <c r="H10" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="J10" s="44" t="str">
+        <f>LEFT(I10,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K10" s="44" t="str">
+        <f>RIGHT(I10,4)</f>
+        <v>2279</v>
+      </c>
+      <c r="L10" s="40">
+        <v>42596</v>
+      </c>
+      <c r="M10" s="40">
+        <f>L10+365</f>
+        <v>42961</v>
+      </c>
+      <c r="N10" s="45">
+        <v>58400</v>
+      </c>
+      <c r="O10" s="46">
+        <f>N10*Pension_Rate</f>
+        <v>5256</v>
+      </c>
+      <c r="P10" s="47">
+        <f>SUM('Staff (2)'!$N10:$O10)</f>
+        <v>63656</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A11" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" s="25" t="str">
+        <f>LOWER(C11&amp;"."&amp;B11&amp;"@pushpin.com")</f>
+        <v>janet.comuntzis@pushpin.com</v>
+      </c>
+      <c r="F11" s="40">
+        <v>39686</v>
+      </c>
+      <c r="G11" s="41">
+        <f ca="1">YEARFRAC(F11,TODAY())</f>
+        <v>11.811111111111112</v>
+      </c>
+      <c r="H11" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="J11" s="44" t="str">
+        <f>LEFT(I11,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K11" s="44" t="str">
+        <f>RIGHT(I11,4)</f>
+        <v>2286</v>
+      </c>
+      <c r="L11" s="40">
+        <v>42658</v>
+      </c>
+      <c r="M11" s="40">
+        <f>L11+365</f>
+        <v>43023</v>
+      </c>
+      <c r="N11" s="45">
+        <v>55800</v>
+      </c>
+      <c r="O11" s="46">
+        <f>N11*Pension_Rate</f>
+        <v>5022</v>
+      </c>
+      <c r="P11" s="47">
+        <f>SUM('Staff (2)'!$N11:$O11)</f>
+        <v>60822</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A12" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="25" t="str">
+        <f>LOWER(C12&amp;"."&amp;B12&amp;"@pushpin.com")</f>
+        <v>sabrina.cole@pushpin.com</v>
+      </c>
+      <c r="F12" s="40">
+        <v>41401</v>
+      </c>
+      <c r="G12" s="41">
+        <f ca="1">YEARFRAC(F12,TODAY())</f>
+        <v>7.1138888888888889</v>
+      </c>
+      <c r="H12" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="J12" s="44" t="str">
+        <f>LEFT(I12,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K12" s="44" t="str">
+        <f>RIGHT(I12,4)</f>
+        <v>2537</v>
+      </c>
+      <c r="L12" s="40">
+        <v>42710</v>
+      </c>
+      <c r="M12" s="40">
+        <f>L12+365</f>
+        <v>43075</v>
+      </c>
+      <c r="N12" s="45">
+        <v>45100</v>
+      </c>
+      <c r="O12" s="46">
+        <f>N12*Pension_Rate</f>
+        <v>4059</v>
+      </c>
+      <c r="P12" s="47">
+        <f>SUM('Staff (2)'!$N12:$O12)</f>
+        <v>49159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A13" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" s="25" t="str">
+        <f>LOWER(C13&amp;"."&amp;B13&amp;"@pushpin.com")</f>
+        <v>elizabeth.clark@pushpin.com</v>
+      </c>
+      <c r="F13" s="40">
+        <v>42874</v>
+      </c>
+      <c r="G13" s="41">
+        <f ca="1">YEARFRAC(F13,TODAY())</f>
+        <v>3.0805555555555557</v>
+      </c>
+      <c r="H13" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="J13" s="44" t="str">
+        <f>LEFT(I13,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K13" s="44" t="str">
+        <f>RIGHT(I13,4)</f>
+        <v>2414</v>
+      </c>
+      <c r="L13" s="40">
+        <v>42720</v>
+      </c>
+      <c r="M13" s="40">
+        <f>L13+365</f>
+        <v>43085</v>
+      </c>
+      <c r="N13" s="45">
+        <v>37000</v>
+      </c>
+      <c r="O13" s="46">
+        <f>N13*Pension_Rate</f>
+        <v>3330</v>
+      </c>
+      <c r="P13" s="47">
+        <f>SUM('Staff (2)'!$N13:$O13)</f>
+        <v>40330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="29" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="39"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="I14" s="43"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="45">
+        <f>SUBTOTAL(9,N9:N13)</f>
+        <v>255500</v>
+      </c>
+      <c r="O14" s="46">
+        <f>SUBTOTAL(9,O9:O13)</f>
+        <v>22995</v>
+      </c>
+      <c r="P14" s="47">
+        <f>SUBTOTAL(9,P9:P13)</f>
+        <v>278495</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A15" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E15" s="25" t="str">
+        <f>LOWER(C15&amp;"."&amp;B15&amp;"@pushpin.com")</f>
+        <v>joe.carol@pushpin.com</v>
+      </c>
+      <c r="F15" s="40">
+        <v>36923</v>
+      </c>
+      <c r="G15" s="41">
+        <f ca="1">YEARFRAC(F15,TODAY())</f>
+        <v>19.380555555555556</v>
+      </c>
+      <c r="H15" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="J15" s="44" t="str">
+        <f>LEFT(I15,2)</f>
+        <v>01</v>
+      </c>
+      <c r="K15" s="44" t="str">
+        <f>RIGHT(I15,4)</f>
+        <v>2321</v>
+      </c>
+      <c r="L15" s="40">
+        <v>42817</v>
+      </c>
+      <c r="M15" s="40">
+        <f>L15+365</f>
+        <v>43182</v>
+      </c>
+      <c r="N15" s="45">
+        <v>101400</v>
+      </c>
+      <c r="O15" s="46">
+        <f>N15*Pension_Rate</f>
+        <v>9126</v>
+      </c>
+      <c r="P15" s="47">
+        <f>SUM('Staff (2)'!$N15:$O15)</f>
+        <v>110526</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A16" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E16" s="25" t="str">
+        <f>LOWER(C16&amp;"."&amp;B16&amp;"@pushpin.com")</f>
+        <v>mei.wang@pushpin.com</v>
+      </c>
+      <c r="F16" s="40">
+        <v>40188</v>
+      </c>
+      <c r="G16" s="41">
+        <f ca="1">YEARFRAC(F16,TODAY())</f>
+        <v>10.438888888888888</v>
+      </c>
+      <c r="H16" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="J16" s="44" t="str">
+        <f>LEFT(I16,2)</f>
+        <v>01</v>
+      </c>
+      <c r="K16" s="44" t="str">
+        <f>RIGHT(I16,4)</f>
+        <v>2783</v>
+      </c>
+      <c r="L16" s="40">
+        <v>42544</v>
+      </c>
+      <c r="M16" s="40">
+        <f>L16+365</f>
+        <v>42909</v>
+      </c>
+      <c r="N16" s="45">
+        <v>96400</v>
+      </c>
+      <c r="O16" s="46">
+        <f>N16*Pension_Rate</f>
+        <v>8676</v>
+      </c>
+      <c r="P16" s="47">
+        <f>SUM('Staff (2)'!$N16:$O16)</f>
+        <v>105076</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="39"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="49" t="s">
+        <v>178</v>
+      </c>
+      <c r="I17" s="43"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="45">
+        <f>SUBTOTAL(9,N15:N16)</f>
+        <v>197800</v>
+      </c>
+      <c r="O17" s="46">
+        <f>SUBTOTAL(9,O15:O16)</f>
+        <v>17802</v>
+      </c>
+      <c r="P17" s="47">
+        <f>SUBTOTAL(9,P15:P16)</f>
+        <v>215602</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A18" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E18" s="25" t="str">
+        <f>LOWER(C18&amp;"."&amp;B18&amp;"@pushpin.com")</f>
+        <v>jim.chaffee@pushpin.com</v>
+      </c>
+      <c r="F18" s="40">
+        <v>41787</v>
+      </c>
+      <c r="G18" s="41">
+        <f ca="1">YEARFRAC(F18,TODAY())</f>
+        <v>6.0555555555555554</v>
+      </c>
+      <c r="H18" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="J18" s="44" t="str">
+        <f>LEFT(I18,2)</f>
+        <v>03</v>
+      </c>
+      <c r="K18" s="44" t="str">
+        <f>RIGHT(I18,4)</f>
+        <v>2432</v>
+      </c>
+      <c r="L18" s="40">
+        <v>42804</v>
+      </c>
+      <c r="M18" s="40">
+        <f>L18+365</f>
+        <v>43169</v>
+      </c>
+      <c r="N18" s="45">
+        <v>42100</v>
+      </c>
+      <c r="O18" s="46">
+        <f>N18*Pension_Rate</f>
+        <v>3789</v>
+      </c>
+      <c r="P18" s="47">
+        <f>SUM('Staff (2)'!$N18:$O18)</f>
+        <v>45889</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="39"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="I19" s="43"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="45">
+        <f>SUBTOTAL(9,N18:N18)</f>
+        <v>42100</v>
+      </c>
+      <c r="O19" s="46">
+        <f>SUBTOTAL(9,O18:O18)</f>
+        <v>3789</v>
+      </c>
+      <c r="P19" s="47">
+        <f>SUBTOTAL(9,P18:P18)</f>
+        <v>45889</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A20" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" s="25" t="str">
+        <f>LOWER(C20&amp;"."&amp;B20&amp;"@pushpin.com")</f>
+        <v>uma.chaudri@pushpin.com</v>
+      </c>
+      <c r="F20" s="40">
+        <v>40994</v>
+      </c>
+      <c r="G20" s="41">
+        <f ca="1">YEARFRAC(F20,TODAY())</f>
+        <v>8.2277777777777779</v>
+      </c>
+      <c r="H20" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="J20" s="44" t="str">
+        <f>LEFT(I20,2)</f>
+        <v>03</v>
+      </c>
+      <c r="K20" s="44" t="str">
+        <f>RIGHT(I20,4)</f>
+        <v>2134</v>
+      </c>
+      <c r="L20" s="40">
+        <v>42776</v>
+      </c>
+      <c r="M20" s="40">
+        <f>L20+365</f>
+        <v>43141</v>
+      </c>
+      <c r="N20" s="45">
+        <v>63200</v>
+      </c>
+      <c r="O20" s="46">
+        <f>N20*Pension_Rate</f>
+        <v>5688</v>
+      </c>
+      <c r="P20" s="47">
+        <f>SUM('Staff (2)'!$N20:$O20)</f>
+        <v>68888</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A21" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E21" s="25" t="str">
+        <f>LOWER(C21&amp;"."&amp;B21&amp;"@pushpin.com")</f>
+        <v>carlos.martinez@pushpin.com</v>
+      </c>
+      <c r="F21" s="40">
+        <v>42229</v>
+      </c>
+      <c r="G21" s="41">
+        <f ca="1">YEARFRAC(F21,TODAY())</f>
+        <v>4.8472222222222223</v>
+      </c>
+      <c r="H21" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="J21" s="44" t="str">
+        <f>LEFT(I21,2)</f>
+        <v>03</v>
+      </c>
+      <c r="K21" s="44" t="str">
+        <f>RIGHT(I21,4)</f>
+        <v>2764</v>
+      </c>
+      <c r="L21" s="40">
+        <v>42845</v>
+      </c>
+      <c r="M21" s="40">
+        <f>L21+365</f>
+        <v>43210</v>
+      </c>
+      <c r="N21" s="45">
+        <v>47900</v>
+      </c>
+      <c r="O21" s="46">
+        <f>N21*Pension_Rate</f>
+        <v>4311</v>
+      </c>
+      <c r="P21" s="47">
+        <f>SUM('Staff (2)'!$N21:$O21)</f>
+        <v>52211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A22" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" s="25" t="str">
+        <f>LOWER(C22&amp;"."&amp;B22&amp;"@pushpin.com")</f>
+        <v>sean.sanders@pushpin.com</v>
+      </c>
+      <c r="F22" s="40">
+        <v>42691</v>
+      </c>
+      <c r="G22" s="41">
+        <f ca="1">YEARFRAC(F22,TODAY())</f>
+        <v>3.5861111111111112</v>
+      </c>
+      <c r="H22" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="J22" s="44" t="str">
+        <f>LEFT(I22,2)</f>
+        <v>03</v>
+      </c>
+      <c r="K22" s="44" t="str">
+        <f>RIGHT(I22,4)</f>
+        <v>2765</v>
+      </c>
+      <c r="L22" s="40">
+        <v>42566</v>
+      </c>
+      <c r="M22" s="40">
+        <f>L22+365</f>
+        <v>42931</v>
+      </c>
+      <c r="N22" s="45">
+        <v>38600</v>
+      </c>
+      <c r="O22" s="46">
+        <f>N22*Pension_Rate</f>
+        <v>3474</v>
+      </c>
+      <c r="P22" s="47">
+        <f>SUM('Staff (2)'!$N22:$O22)</f>
+        <v>42074</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="29" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="39"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="I23" s="43"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="45">
+        <f>SUBTOTAL(9,N20:N22)</f>
+        <v>149700</v>
+      </c>
+      <c r="O23" s="46">
+        <f>SUBTOTAL(9,O20:O22)</f>
+        <v>13473</v>
+      </c>
+      <c r="P23" s="47">
+        <f>SUBTOTAL(9,P20:P22)</f>
+        <v>163173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A24" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E24" s="25" t="str">
+        <f>LOWER(C24&amp;"."&amp;B24&amp;"@pushpin.com")</f>
+        <v>eric.chung@pushpin.com</v>
+      </c>
+      <c r="F24" s="40">
+        <v>36949</v>
+      </c>
+      <c r="G24" s="41">
+        <f ca="1">YEARFRAC(F24,TODAY())</f>
+        <v>19.308333333333334</v>
+      </c>
+      <c r="H24" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="I24" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="J24" s="44" t="str">
+        <f>LEFT(I24,2)</f>
+        <v>03</v>
+      </c>
+      <c r="K24" s="44" t="str">
+        <f>RIGHT(I24,4)</f>
+        <v>2796</v>
+      </c>
+      <c r="L24" s="40">
+        <v>42731</v>
+      </c>
+      <c r="M24" s="40">
+        <f>L24+365</f>
+        <v>43096</v>
+      </c>
+      <c r="N24" s="45">
+        <v>70300</v>
+      </c>
+      <c r="O24" s="46">
+        <f>N24*Pension_Rate</f>
+        <v>6327</v>
+      </c>
+      <c r="P24" s="47">
+        <f>SUM('Staff (2)'!$N24:$O24)</f>
+        <v>76627</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A25" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E25" s="25" t="str">
+        <f>LOWER(C25&amp;"."&amp;B25&amp;"@pushpin.com")</f>
+        <v>elizabeth.chu@pushpin.com</v>
+      </c>
+      <c r="F25" s="40">
+        <v>40220</v>
+      </c>
+      <c r="G25" s="41">
+        <f ca="1">YEARFRAC(F25,TODAY())</f>
+        <v>10.352777777777778</v>
+      </c>
+      <c r="H25" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="J25" s="44" t="str">
+        <f>LEFT(I25,2)</f>
+        <v>01</v>
+      </c>
+      <c r="K25" s="44" t="str">
+        <f>RIGHT(I25,4)</f>
+        <v>2425</v>
+      </c>
+      <c r="L25" s="40">
+        <v>42761</v>
+      </c>
+      <c r="M25" s="40">
+        <f>L25+365</f>
+        <v>43126</v>
+      </c>
+      <c r="N25" s="45">
+        <v>48400</v>
+      </c>
+      <c r="O25" s="46">
+        <f>N25*Pension_Rate</f>
+        <v>4356</v>
+      </c>
+      <c r="P25" s="47">
+        <f>SUM('Staff (2)'!$N25:$O25)</f>
+        <v>52756</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A26" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E26" s="25" t="str">
+        <f>LOWER(C26&amp;"."&amp;B26&amp;"@pushpin.com")</f>
+        <v>tina.desiato@pushpin.com</v>
+      </c>
+      <c r="F26" s="40">
+        <v>41175</v>
+      </c>
+      <c r="G26" s="41">
+        <f ca="1">YEARFRAC(F26,TODAY())</f>
+        <v>7.7361111111111107</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="J26" s="44" t="str">
+        <f>LEFT(I26,2)</f>
+        <v>01</v>
+      </c>
+      <c r="K26" s="44" t="str">
+        <f>RIGHT(I26,4)</f>
+        <v>2358</v>
+      </c>
+      <c r="L26" s="40">
+        <v>42652</v>
+      </c>
+      <c r="M26" s="40">
+        <f>L26+365</f>
+        <v>43017</v>
+      </c>
+      <c r="N26" s="45">
+        <v>51700</v>
+      </c>
+      <c r="O26" s="46">
+        <f>N26*Pension_Rate</f>
+        <v>4653</v>
+      </c>
+      <c r="P26" s="47">
+        <f>SUM('Staff (2)'!$N26:$O26)</f>
+        <v>56353</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A27" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E27" s="25" t="str">
+        <f>LOWER(C27&amp;"."&amp;B27&amp;"@pushpin.com")</f>
+        <v>bob.decker@pushpin.com</v>
+      </c>
+      <c r="F27" s="40">
+        <v>41210</v>
+      </c>
+      <c r="G27" s="41">
+        <f ca="1">YEARFRAC(F27,TODAY())</f>
+        <v>7.6388888888888893</v>
+      </c>
+      <c r="H27" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="I27" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="J27" s="44" t="str">
+        <f>LEFT(I27,2)</f>
+        <v>01</v>
+      </c>
+      <c r="K27" s="44" t="str">
+        <f>RIGHT(I27,4)</f>
+        <v>2086</v>
+      </c>
+      <c r="L27" s="40">
+        <v>42656</v>
+      </c>
+      <c r="M27" s="40">
+        <f>L27+365</f>
+        <v>43021</v>
+      </c>
+      <c r="N27" s="45">
+        <v>49600</v>
+      </c>
+      <c r="O27" s="46">
+        <f>N27*Pension_Rate</f>
+        <v>4464</v>
+      </c>
+      <c r="P27" s="47">
+        <f>SUM('Staff (2)'!$N27:$O27)</f>
+        <v>54064</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A28" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E28" s="25" t="str">
+        <f>LOWER(C28&amp;"."&amp;B28&amp;"@pushpin.com")</f>
+        <v>mark.ellis@pushpin.com</v>
+      </c>
+      <c r="F28" s="40">
+        <v>42371</v>
+      </c>
+      <c r="G28" s="41">
+        <f ca="1">YEARFRAC(F28,TODAY())</f>
+        <v>4.4611111111111112</v>
+      </c>
+      <c r="H28" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="I28" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="J28" s="44" t="str">
+        <f>LEFT(I28,2)</f>
+        <v>03</v>
+      </c>
+      <c r="K28" s="44" t="str">
+        <f>RIGHT(I28,4)</f>
+        <v>2482</v>
+      </c>
+      <c r="L28" s="40">
+        <v>42619</v>
+      </c>
+      <c r="M28" s="40">
+        <f>L28+365</f>
+        <v>42984</v>
+      </c>
+      <c r="N28" s="45">
+        <v>58500</v>
+      </c>
+      <c r="O28" s="46">
+        <f>N28*Pension_Rate</f>
+        <v>5265</v>
+      </c>
+      <c r="P28" s="47">
+        <f>SUM('Staff (2)'!$N28:$O28)</f>
+        <v>63765</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="39"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="I29" s="43"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="45">
+        <f>SUBTOTAL(9,N24:N28)</f>
+        <v>278500</v>
+      </c>
+      <c r="O29" s="46">
+        <f>SUBTOTAL(9,O24:O28)</f>
+        <v>25065</v>
+      </c>
+      <c r="P29" s="47">
+        <f>SUBTOTAL(9,P24:P28)</f>
+        <v>303565</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A30" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E30" s="25" t="str">
+        <f>LOWER(C30&amp;"."&amp;B30&amp;"@pushpin.com")</f>
+        <v>william.grey@pushpin.com</v>
+      </c>
+      <c r="F30" s="48">
+        <v>42933</v>
+      </c>
+      <c r="G30" s="41">
+        <f ca="1">YEARFRAC(F30,TODAY())</f>
+        <v>2.9194444444444443</v>
+      </c>
+      <c r="H30" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="I30" s="43"/>
+      <c r="J30" s="44" t="str">
+        <f>LEFT(I30,2)</f>
+        <v/>
+      </c>
+      <c r="K30" s="44" t="str">
+        <f>RIGHT(I30,4)</f>
+        <v/>
+      </c>
+      <c r="L30" s="48">
+        <v>42933</v>
+      </c>
+      <c r="M30" s="48">
+        <f>L30+365</f>
+        <v>43298</v>
+      </c>
+      <c r="N30" s="45">
+        <v>97000</v>
+      </c>
+      <c r="O30" s="46">
+        <f>N30*Pension_Rate</f>
+        <v>8730</v>
+      </c>
+      <c r="P30" s="47">
+        <f>SUM('Staff (2)'!$N30:$O30)</f>
+        <v>105730</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="39"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="49" t="s">
+        <v>182</v>
+      </c>
+      <c r="I31" s="43"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="45">
+        <f>SUBTOTAL(9,N30:N30)</f>
+        <v>97000</v>
+      </c>
+      <c r="O31" s="46">
+        <f>SUBTOTAL(9,O30:O30)</f>
+        <v>8730</v>
+      </c>
+      <c r="P31" s="47">
+        <f>SUBTOTAL(9,P30:P30)</f>
+        <v>105730</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A32" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E32" s="25" t="str">
+        <f>LOWER(C32&amp;"."&amp;B32&amp;"@pushpin.com")</f>
+        <v>daniel.flanders@pushpin.com</v>
+      </c>
+      <c r="F32" s="40">
+        <v>37510</v>
+      </c>
+      <c r="G32" s="41">
+        <f ca="1">YEARFRAC(F32,TODAY())</f>
+        <v>17.769444444444446</v>
+      </c>
+      <c r="H32" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="J32" s="44" t="str">
+        <f>LEFT(I32,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K32" s="44" t="str">
+        <f>RIGHT(I32,4)</f>
+        <v>2639</v>
+      </c>
+      <c r="L32" s="40">
+        <v>42590</v>
+      </c>
+      <c r="M32" s="40">
+        <f>L32+365</f>
+        <v>42955</v>
+      </c>
+      <c r="N32" s="45">
+        <v>68800</v>
+      </c>
+      <c r="O32" s="46">
+        <f>N32*Pension_Rate</f>
+        <v>6192</v>
+      </c>
+      <c r="P32" s="47">
+        <f>SUM('Staff (2)'!$N32:$O32)</f>
+        <v>74992</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A33" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E33" s="25" t="str">
+        <f>LOWER(C33&amp;"."&amp;B33&amp;"@pushpin.com")</f>
+        <v>mary.ferris@pushpin.com</v>
+      </c>
+      <c r="F33" s="40">
+        <v>38548</v>
+      </c>
+      <c r="G33" s="41">
+        <f ca="1">YEARFRAC(F33,TODAY())</f>
+        <v>14.925000000000001</v>
+      </c>
+      <c r="H33" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="J33" s="44" t="str">
+        <f>LEFT(I33,2)</f>
+        <v>03</v>
+      </c>
+      <c r="K33" s="44" t="str">
+        <f>RIGHT(I33,4)</f>
+        <v>2392</v>
+      </c>
+      <c r="L33" s="40">
+        <v>42598</v>
+      </c>
+      <c r="M33" s="40">
+        <f>L33+365</f>
+        <v>42963</v>
+      </c>
+      <c r="N33" s="45">
+        <v>62900</v>
+      </c>
+      <c r="O33" s="46">
+        <f>N33*Pension_Rate</f>
+        <v>5661</v>
+      </c>
+      <c r="P33" s="47">
+        <f>SUM('Staff (2)'!$N33:$O33)</f>
+        <v>68561</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A34" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E34" s="25" t="str">
+        <f>LOWER(C34&amp;"."&amp;B34&amp;"@pushpin.com")</f>
+        <v>tina.carlton@pushpin.com</v>
+      </c>
+      <c r="F34" s="40">
+        <v>38798</v>
+      </c>
+      <c r="G34" s="41">
+        <f ca="1">YEARFRAC(F34,TODAY())</f>
+        <v>14.238888888888889</v>
+      </c>
+      <c r="H34" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I34" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="J34" s="44" t="str">
+        <f>LEFT(I34,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K34" s="44" t="str">
+        <f>RIGHT(I34,4)</f>
+        <v>2699</v>
+      </c>
+      <c r="L34" s="40">
+        <v>42825</v>
+      </c>
+      <c r="M34" s="40">
+        <f>L34+365</f>
+        <v>43190</v>
+      </c>
+      <c r="N34" s="45">
+        <v>59200</v>
+      </c>
+      <c r="O34" s="46">
+        <f>N34*Pension_Rate</f>
+        <v>5328</v>
+      </c>
+      <c r="P34" s="47">
+        <f>SUM('Staff (2)'!$N34:$O34)</f>
+        <v>64528</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A35" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E35" s="25" t="str">
+        <f>LOWER(C35&amp;"."&amp;B35&amp;"@pushpin.com")</f>
+        <v>stevie.bacata@pushpin.com</v>
+      </c>
+      <c r="F35" s="40">
+        <v>39551</v>
+      </c>
+      <c r="G35" s="41">
+        <f ca="1">YEARFRAC(F35,TODAY())</f>
+        <v>12.180555555555555</v>
+      </c>
+      <c r="H35" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I35" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="J35" s="44" t="str">
+        <f>LEFT(I35,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K35" s="44" t="str">
+        <f>RIGHT(I35,4)</f>
+        <v>2635</v>
+      </c>
+      <c r="L35" s="40">
+        <v>42507</v>
+      </c>
+      <c r="M35" s="40">
+        <f>L35+365</f>
+        <v>42872</v>
+      </c>
+      <c r="N35" s="45">
+        <v>58200</v>
+      </c>
+      <c r="O35" s="46">
+        <f>N35*Pension_Rate</f>
+        <v>5238</v>
+      </c>
+      <c r="P35" s="47">
+        <f>SUM('Staff (2)'!$N35:$O35)</f>
+        <v>63438</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A36" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E36" s="25" t="str">
+        <f>LOWER(C36&amp;"."&amp;B36&amp;"@pushpin.com")</f>
+        <v>mihael.khan@pushpin.com</v>
+      </c>
+      <c r="F36" s="40">
+        <v>40160</v>
+      </c>
+      <c r="G36" s="41">
+        <f ca="1">YEARFRAC(F36,TODAY())</f>
+        <v>10.513888888888889</v>
+      </c>
+      <c r="H36" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I36" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="J36" s="44" t="str">
+        <f>LEFT(I36,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K36" s="44" t="str">
+        <f>RIGHT(I36,4)</f>
+        <v>2294</v>
+      </c>
+      <c r="L36" s="40">
+        <v>42566</v>
+      </c>
+      <c r="M36" s="40">
+        <f>L36+365</f>
+        <v>42931</v>
+      </c>
+      <c r="N36" s="45">
+        <v>55500</v>
+      </c>
+      <c r="O36" s="46">
+        <f>N36*Pension_Rate</f>
+        <v>4995</v>
+      </c>
+      <c r="P36" s="47">
+        <f>SUM('Staff (2)'!$N36:$O36)</f>
+        <v>60495</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A37" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E37" s="25" t="str">
+        <f>LOWER(C37&amp;"."&amp;B37&amp;"@pushpin.com")</f>
+        <v>samantha.chairs@pushpin.com</v>
+      </c>
+      <c r="F37" s="40">
+        <v>40595</v>
+      </c>
+      <c r="G37" s="41">
+        <f ca="1">YEARFRAC(F37,TODAY())</f>
+        <v>9.3249999999999993</v>
+      </c>
+      <c r="H37" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I37" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="J37" s="44" t="str">
+        <f>LEFT(I37,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K37" s="44" t="str">
+        <f>RIGHT(I37,4)</f>
+        <v>2962</v>
+      </c>
+      <c r="L37" s="40">
+        <v>42801</v>
+      </c>
+      <c r="M37" s="40">
+        <f>L37+365</f>
+        <v>43166</v>
+      </c>
+      <c r="N37" s="45">
+        <v>59300</v>
+      </c>
+      <c r="O37" s="46">
+        <f>N37*Pension_Rate</f>
+        <v>5337</v>
+      </c>
+      <c r="P37" s="47">
+        <f>SUM('Staff (2)'!$N37:$O37)</f>
+        <v>64637</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A38" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E38" s="25" t="str">
+        <f>LOWER(C38&amp;"."&amp;B38&amp;"@pushpin.com")</f>
+        <v>natasha.song@pushpin.com</v>
+      </c>
+      <c r="F38" s="40">
+        <v>40713</v>
+      </c>
+      <c r="G38" s="41">
+        <f ca="1">YEARFRAC(F38,TODAY())</f>
+        <v>8.9972222222222218</v>
+      </c>
+      <c r="H38" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I38" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="J38" s="44" t="str">
+        <f>LEFT(I38,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K38" s="44" t="str">
+        <f>RIGHT(I38,4)</f>
+        <v>2578</v>
+      </c>
+      <c r="L38" s="40">
+        <v>42552</v>
+      </c>
+      <c r="M38" s="40">
+        <f>L38+365</f>
+        <v>42917</v>
+      </c>
+      <c r="N38" s="45">
+        <v>56000</v>
+      </c>
+      <c r="O38" s="46">
+        <f>N38*Pension_Rate</f>
+        <v>5040</v>
+      </c>
+      <c r="P38" s="47">
+        <f>SUM('Staff (2)'!$N38:$O38)</f>
+        <v>61040</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A39" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E39" s="25" t="str">
+        <f>LOWER(C39&amp;"."&amp;B39&amp;"@pushpin.com")</f>
+        <v>charlie.bui@pushpin.com</v>
+      </c>
+      <c r="F39" s="40">
+        <v>41903</v>
+      </c>
+      <c r="G39" s="41">
+        <f ca="1">YEARFRAC(F39,TODAY())</f>
+        <v>5.7416666666666663</v>
+      </c>
+      <c r="H39" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I39" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="J39" s="44" t="str">
+        <f>LEFT(I39,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K39" s="44" t="str">
+        <f>RIGHT(I39,4)</f>
+        <v>2694</v>
+      </c>
+      <c r="L39" s="40">
+        <v>42828</v>
+      </c>
+      <c r="M39" s="40">
+        <f>L39+365</f>
+        <v>43193</v>
+      </c>
+      <c r="N39" s="45">
+        <v>54700</v>
+      </c>
+      <c r="O39" s="46">
+        <f>N39*Pension_Rate</f>
+        <v>4923</v>
+      </c>
+      <c r="P39" s="47">
+        <f>SUM('Staff (2)'!$N39:$O39)</f>
+        <v>59623</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A40" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" s="25" t="str">
+        <f>LOWER(C40&amp;"."&amp;B40&amp;"@pushpin.com")</f>
+        <v>connor.betts@pushpin.com</v>
+      </c>
+      <c r="F40" s="40">
+        <v>41956</v>
+      </c>
+      <c r="G40" s="41">
+        <f ca="1">YEARFRAC(F40,TODAY())</f>
+        <v>5.5972222222222223</v>
+      </c>
+      <c r="H40" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I40" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="J40" s="44" t="str">
+        <f>LEFT(I40,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K40" s="44" t="str">
+        <f>RIGHT(I40,4)</f>
+        <v>2347</v>
+      </c>
+      <c r="L40" s="40">
+        <v>42848</v>
+      </c>
+      <c r="M40" s="40">
+        <f>L40+365</f>
+        <v>43213</v>
+      </c>
+      <c r="N40" s="45">
+        <v>52600</v>
+      </c>
+      <c r="O40" s="46">
+        <f>N40*Pension_Rate</f>
+        <v>4734</v>
+      </c>
+      <c r="P40" s="47">
+        <f>SUM('Staff (2)'!$N40:$O40)</f>
+        <v>57334</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A41" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E41" s="25" t="str">
+        <f>LOWER(C41&amp;"."&amp;B41&amp;"@pushpin.com")</f>
+        <v>aanya.zhang@pushpin.com</v>
+      </c>
+      <c r="F41" s="40">
+        <v>42002</v>
+      </c>
+      <c r="G41" s="41">
+        <f ca="1">YEARFRAC(F41,TODAY())</f>
+        <v>5.4694444444444441</v>
+      </c>
+      <c r="H41" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I41" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="J41" s="44" t="str">
+        <f>LEFT(I41,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K41" s="44" t="str">
+        <f>RIGHT(I41,4)</f>
+        <v>2793</v>
+      </c>
+      <c r="L41" s="40">
+        <v>42540</v>
+      </c>
+      <c r="M41" s="40">
+        <f>L41+365</f>
+        <v>42905</v>
+      </c>
+      <c r="N41" s="45">
+        <v>46500</v>
+      </c>
+      <c r="O41" s="46">
+        <f>N41*Pension_Rate</f>
+        <v>4185</v>
+      </c>
+      <c r="P41" s="47">
+        <f>SUM('Staff (2)'!$N41:$O41)</f>
+        <v>50685</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A42" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E42" s="25" t="str">
+        <f>LOWER(C42&amp;"."&amp;B42&amp;"@pushpin.com")</f>
+        <v>leighton.forrest@pushpin.com</v>
+      </c>
+      <c r="F42" s="40">
+        <v>42120</v>
+      </c>
+      <c r="G42" s="41">
+        <f ca="1">YEARFRAC(F42,TODAY())</f>
+        <v>5.1444444444444448</v>
+      </c>
+      <c r="H42" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I42" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="J42" s="44" t="str">
+        <f>LEFT(I42,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K42" s="44" t="str">
+        <f>RIGHT(I42,4)</f>
+        <v>2284</v>
+      </c>
+      <c r="L42" s="40">
+        <v>42586</v>
+      </c>
+      <c r="M42" s="40">
+        <f>L42+365</f>
+        <v>42951</v>
+      </c>
+      <c r="N42" s="45">
+        <v>56200</v>
+      </c>
+      <c r="O42" s="46">
+        <f>N42*Pension_Rate</f>
+        <v>5058</v>
+      </c>
+      <c r="P42" s="47">
+        <f>SUM('Staff (2)'!$N42:$O42)</f>
+        <v>61258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A43" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E43" s="25" t="str">
+        <f>LOWER(C43&amp;"."&amp;B43&amp;"@pushpin.com")</f>
+        <v>peter.staples@pushpin.com</v>
+      </c>
+      <c r="F43" s="40">
+        <v>42321</v>
+      </c>
+      <c r="G43" s="41">
+        <f ca="1">YEARFRAC(F43,TODAY())</f>
+        <v>4.5972222222222223</v>
+      </c>
+      <c r="H43" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I43" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="J43" s="44" t="str">
+        <f>LEFT(I43,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K43" s="44" t="str">
+        <f>RIGHT(I43,4)</f>
+        <v>2654</v>
+      </c>
+      <c r="L43" s="40">
+        <v>42551</v>
+      </c>
+      <c r="M43" s="40">
+        <f>L43+365</f>
+        <v>42916</v>
+      </c>
+      <c r="N43" s="45">
+        <v>49600</v>
+      </c>
+      <c r="O43" s="46">
+        <f>N43*Pension_Rate</f>
+        <v>4464</v>
+      </c>
+      <c r="P43" s="47">
+        <f>SUM('Staff (2)'!$N43:$O43)</f>
+        <v>54064</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A44" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E44" s="25" t="str">
+        <f>LOWER(C44&amp;"."&amp;B44&amp;"@pushpin.com")</f>
+        <v>radhya.senome@pushpin.com</v>
+      </c>
+      <c r="F44" s="40">
+        <v>42324</v>
+      </c>
+      <c r="G44" s="41">
+        <f ca="1">YEARFRAC(F44,TODAY())</f>
+        <v>4.5888888888888886</v>
+      </c>
+      <c r="H44" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I44" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="J44" s="44" t="str">
+        <f>LEFT(I44,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K44" s="44" t="str">
+        <f>RIGHT(I44,4)</f>
+        <v>2260</v>
+      </c>
+      <c r="L44" s="40">
+        <v>42563</v>
+      </c>
+      <c r="M44" s="40">
+        <f>L44+365</f>
+        <v>42928</v>
+      </c>
+      <c r="N44" s="45">
+        <v>35600</v>
+      </c>
+      <c r="O44" s="46">
+        <f>N44*Pension_Rate</f>
+        <v>3204</v>
+      </c>
+      <c r="P44" s="47">
+        <f>SUM('Staff (2)'!$N44:$O44)</f>
+        <v>38804</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A45" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E45" s="25" t="str">
+        <f>LOWER(C45&amp;"."&amp;B45&amp;"@pushpin.com")</f>
+        <v>yvette.biti@pushpin.com</v>
+      </c>
+      <c r="F45" s="40">
+        <v>42384</v>
+      </c>
+      <c r="G45" s="41">
+        <f ca="1">YEARFRAC(F45,TODAY())</f>
+        <v>4.4249999999999998</v>
+      </c>
+      <c r="H45" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I45" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="J45" s="44" t="str">
+        <f>LEFT(I45,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K45" s="44" t="str">
+        <f>RIGHT(I45,4)</f>
+        <v>2589</v>
+      </c>
+      <c r="L45" s="40">
+        <v>42839</v>
+      </c>
+      <c r="M45" s="40">
+        <f>L45+365</f>
+        <v>43204</v>
+      </c>
+      <c r="N45" s="45">
+        <v>51400</v>
+      </c>
+      <c r="O45" s="46">
+        <f>N45*Pension_Rate</f>
+        <v>4626</v>
+      </c>
+      <c r="P45" s="47">
+        <f>SUM('Staff (2)'!$N45:$O45)</f>
+        <v>56026</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+      <c r="A46" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E46" s="25" t="str">
+        <f>LOWER(C46&amp;"."&amp;B46&amp;"@pushpin.com")</f>
+        <v>phoebe.gour@pushpin.com</v>
+      </c>
+      <c r="F46" s="40">
+        <v>42721</v>
+      </c>
+      <c r="G46" s="41">
+        <f ca="1">YEARFRAC(F46,TODAY())</f>
+        <v>3.5027777777777778</v>
+      </c>
+      <c r="H46" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="I46" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="J46" s="44" t="str">
+        <f>LEFT(I46,2)</f>
+        <v>02</v>
+      </c>
+      <c r="K46" s="44" t="str">
+        <f>RIGHT(I46,4)</f>
+        <v>2910</v>
+      </c>
+      <c r="L46" s="40">
+        <v>42539</v>
+      </c>
+      <c r="M46" s="40">
+        <f>L46+365</f>
+        <v>42904</v>
+      </c>
+      <c r="N46" s="45">
+        <v>40500</v>
+      </c>
+      <c r="O46" s="46">
+        <f>N46*Pension_Rate</f>
+        <v>3645</v>
+      </c>
+      <c r="P46" s="47">
+        <f>SUM('Staff (2)'!$N46:$O46)</f>
+        <v>44145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="39"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="I47" s="43"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="40"/>
+      <c r="M47" s="40"/>
+      <c r="N47" s="45">
+        <f>SUBTOTAL(9,N32:N46)</f>
+        <v>807000</v>
+      </c>
+      <c r="O47" s="46">
+        <f>SUBTOTAL(9,O32:O46)</f>
+        <v>72630</v>
+      </c>
+      <c r="P47" s="47">
+        <f>SUBTOTAL(9,P32:P46)</f>
+        <v>879630</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A48" s="39"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="41"/>
+      <c r="H48" s="49" t="s">
+        <v>184</v>
+      </c>
+      <c r="I48" s="43"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="44"/>
+      <c r="L48" s="40"/>
+      <c r="M48" s="40"/>
+      <c r="N48" s="45">
+        <f>SUBTOTAL(9,N4:N46)</f>
+        <v>2055400</v>
+      </c>
+      <c r="O48" s="46">
+        <f>SUBTOTAL(9,O4:O46)</f>
+        <v>184986</v>
+      </c>
+      <c r="P48" s="47">
+        <f>SUBTOTAL(9,P4:P46)</f>
+        <v>2240386</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="E50" s="13"/>
+    </row>
+    <row r="51" spans="5:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="E51" s="13"/>
+    </row>
+    <row r="52" spans="5:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="E52" s="13"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="M4:M48">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>M4&lt;TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="75" verticalDpi="75" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>